<commit_message>
added upper case option and multiple receivers supported
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UiPath\Speranta_Cluj_Birthday_List\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF10ECA-CABC-4482-9428-729C46C32662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8800D4-7987-49FA-8CBE-91B02B452066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="3915" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Windows Credential Name where email credential are stored</t>
   </si>
   <si>
-    <t>Email of the receiver</t>
-  </si>
-  <si>
     <t>Subject of email</t>
   </si>
   <si>
@@ -200,6 +197,18 @@
   </si>
   <si>
     <t>Data\Input\SARBATORITI.pptx</t>
+  </si>
+  <si>
+    <t>toUpperCase</t>
+  </si>
+  <si>
+    <t>Email of the receiver
+Multiple addresses Can be added delimited by "';"
+Ex: receiver1;receiver2;receiver3</t>
+  </si>
+  <si>
+    <t>"TRUE" - changes names to upper case
+"FALSE" - no changes to names</t>
   </si>
 </sst>
 </file>
@@ -251,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -259,6 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,19 +638,21 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B3" s="4"/>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C4" t="s">
@@ -649,68 +663,82 @@
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>58</v>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B6" s="4"/>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="41.25" customHeight="1">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
-        <v>53</v>
+      <c r="C9" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
-        <v>57</v>
+      <c r="B10" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>587</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="32.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>